<commit_message>
added 1). ability to drag and drop multiple file uploads to web app; 2). adding flexibility to xbrl context definitions (to phase out contexts.xlsx; 3). updated the sample template to include statement of activities
</commit_message>
<xml_diff>
--- a/static/input_files/acfrs/IXBRL_contexts.xlsx
+++ b/static/input_files/acfrs/IXBRL_contexts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/input_files/afcrs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/static/input_files/acfrs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DCDFB0-FE08-DD4A-BA8D-0EB422490DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68218A7-DBC1-A540-A293-17598DF0C4DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BC8E164B-12CB-F34A-BBDC-A1FC5F180C48}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{BC8E164B-12CB-F34A-BBDC-A1FC5F180C48}"/>
   </bookViews>
   <sheets>
     <sheet name="Statements" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Simple table" sheetId="2" r:id="rId5"/>
     <sheet name="Includes statement of activitie" sheetId="1" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -750,7 +750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6311D72E-A4AE-6346-BE1B-0CFBE5E49588}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1080,13 +1080,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D52A885-67E7-0847-B2EE-FEA644A9BA26}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" customWidth="1"/>
+    <col min="7" max="7" width="25.5" customWidth="1"/>
+    <col min="8" max="8" width="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -1663,7 +1668,7 @@
   <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H24"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>